<commit_message>
make bom clearer and pushed filter code
</commit_message>
<xml_diff>
--- a/Baseline_Shield_BOM.xlsx
+++ b/Baseline_Shield_BOM.xlsx
@@ -192,9 +192,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="171" formatCode="_(&quot;$&quot;* #,##0.000_);_(&quot;$&quot;* \(#,##0.000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -317,7 +318,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="44" fontId="1" fillId="3" borderId="0" xfId="3" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="3" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="3" applyNumberFormat="1"/>
@@ -329,9 +329,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="2"/>
     <xf numFmtId="164" fontId="3" fillId="2" borderId="2" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="44" fontId="1" fillId="3" borderId="0" xfId="5" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="6"/>
-    <xf numFmtId="44" fontId="1" fillId="4" borderId="0" xfId="6" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="1" fillId="4" borderId="0" xfId="6" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="6" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -340,8 +338,11 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="7" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="44" fontId="1" fillId="5" borderId="0" xfId="7" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="1" fillId="5" borderId="0" xfId="7" applyNumberFormat="1"/>
+    <xf numFmtId="171" fontId="1" fillId="3" borderId="0" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="171" fontId="1" fillId="3" borderId="0" xfId="5" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="171" fontId="1" fillId="4" borderId="0" xfId="6" applyNumberFormat="1"/>
+    <xf numFmtId="171" fontId="1" fillId="5" borderId="0" xfId="7" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="20% - Accent4" xfId="6" builtinId="42"/>
@@ -632,7 +633,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -674,37 +675,37 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="8" t="s">
         <v>39</v>
       </c>
       <c r="D2" s="2">
         <v>110</v>
       </c>
-      <c r="E2" s="14">
+      <c r="E2" s="20">
         <v>0.22800000000000001</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="4">
         <f>E2*D2</f>
         <v>25.080000000000002</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="5" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="8" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -713,22 +714,22 @@
       <c r="D3" s="2">
         <v>660</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="19">
         <v>9.2160000000000006E-2</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="4">
         <f>E3*D3</f>
         <v>60.825600000000001</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -740,224 +741,224 @@
       <c r="D4" s="2">
         <v>110</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="19">
         <v>7.8E-2</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="4">
         <f>E4*D4</f>
         <v>8.58</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="5" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="6" t="s">
         <v>15</v>
       </c>
       <c r="D5" s="2">
         <v>660</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="19">
         <v>6.0200000000000002E-3</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="4">
         <f>E5*D5</f>
         <v>3.9732000000000003</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="5" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="7" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="9" t="s">
         <v>19</v>
       </c>
       <c r="D6" s="2">
         <v>220</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="19">
         <v>6.0200000000000002E-3</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="4">
         <f>E6*D6</f>
         <v>1.3244</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="H6" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="13">
         <v>110</v>
       </c>
-      <c r="E7" s="16">
+      <c r="E7" s="21">
         <v>0.19400000000000001</v>
       </c>
-      <c r="F7" s="17">
+      <c r="F7" s="14">
         <f>E7*D7</f>
         <v>21.34</v>
       </c>
-      <c r="G7" s="17" t="s">
+      <c r="G7" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="H7" s="5" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="D8" s="15">
+      <c r="D8" s="13">
         <v>220</v>
       </c>
-      <c r="E8" s="16">
+      <c r="E8" s="21">
         <v>0.36099999999999999</v>
       </c>
-      <c r="F8" s="17">
+      <c r="F8" s="14">
         <f>E8*D8</f>
         <v>79.42</v>
       </c>
-      <c r="G8" s="17" t="s">
+      <c r="G8" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="H8" s="5" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="D9" s="15">
+      <c r="D9" s="13">
         <v>110</v>
       </c>
-      <c r="E9" s="16">
+      <c r="E9" s="21">
         <v>0.29699999999999999</v>
       </c>
-      <c r="F9" s="17">
+      <c r="F9" s="14">
         <f>E9*D9</f>
         <v>32.67</v>
       </c>
-      <c r="G9" s="17" t="s">
+      <c r="G9" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="H9" s="6" t="s">
+      <c r="H9" s="5" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="C10" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="15">
+      <c r="D10" s="13">
         <v>330</v>
       </c>
-      <c r="E10" s="16">
+      <c r="E10" s="21">
         <v>8.6999999999999994E-2</v>
       </c>
-      <c r="F10" s="17">
+      <c r="F10" s="14">
         <f>E10*D10</f>
         <v>28.709999999999997</v>
       </c>
-      <c r="G10" s="17" t="s">
+      <c r="G10" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="H10" s="6" t="s">
+      <c r="H10" s="5" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="20" t="s">
+      <c r="C11" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="19">
+      <c r="D11" s="16">
         <v>110</v>
       </c>
-      <c r="E11" s="21">
+      <c r="E11" s="22">
         <v>1.35</v>
       </c>
-      <c r="F11" s="22">
+      <c r="F11" s="18">
         <f>E11*D11</f>
         <v>148.5</v>
       </c>
-      <c r="G11" s="22" t="s">
+      <c r="G11" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="H11" s="6" t="s">
+      <c r="H11" s="5" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E14" s="11" t="s">
+      <c r="E14" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="F14" s="12">
+      <c r="F14" s="11">
         <f>SUM(F2:F11)</f>
         <v>410.42320000000001</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E15" s="11" t="s">
+      <c r="E15" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="F15" s="12">
+      <c r="F15" s="11">
         <f>F14/100</f>
         <v>4.1042319999999997</v>
       </c>

</xml_diff>